<commit_message>
Randomized subjects, body, senderName
</commit_message>
<xml_diff>
--- a/receivers.xlsx
+++ b/receivers.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\code_files\Hunter Local\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="J:\programming and stuff\Hunter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FCBBCF5-719C-474D-8845-D3A626488F29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38460" yWindow="2595" windowWidth="15375" windowHeight="11295" xr2:uid="{F4ED9135-05F0-4936-AE87-A8F06421BD50}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7800"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,33 +24,63 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
-  <si>
-    <t>test@gmail.com</t>
-  </si>
-  <si>
-    <t>bacchan.amit69@rekha.com</t>
-  </si>
-  <si>
-    <t>testedBrat@yahoo.com</t>
-  </si>
-  <si>
-    <t>pirates009@hotmail.com</t>
-  </si>
-  <si>
-    <t>xchat@yahoo.com</t>
-  </si>
-  <si>
-    <t>tweet59@gmail.com</t>
-  </si>
-  <si>
-    <t>reddit@t.com</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+  <si>
+    <t>ajaygoel999@gmail.com</t>
+  </si>
+  <si>
+    <t>test@chromecompete.com</t>
+  </si>
+  <si>
+    <t>ajay@ajaygoel.net</t>
+  </si>
+  <si>
+    <t>test@ajaygoel.org</t>
+  </si>
+  <si>
+    <t>me@dropboxslideshow.com</t>
+  </si>
+  <si>
+    <t>test@wordzen.com</t>
+  </si>
+  <si>
+    <t>rajgoel8477@gmail.com</t>
+  </si>
+  <si>
+    <t>rajanderson8477@gmail.com</t>
+  </si>
+  <si>
+    <t>rajwilson8477@gmail.com</t>
+  </si>
+  <si>
+    <t>briansmith8477@gmail.com</t>
+  </si>
+  <si>
+    <t>oliviasmith8477@gmail.com</t>
+  </si>
+  <si>
+    <t>ashsmith8477@gmail.com</t>
+  </si>
+  <si>
+    <t>shellysmith8477@gmail.com</t>
+  </si>
+  <si>
+    <t>ajay@madsciencekidz.com</t>
+  </si>
+  <si>
+    <t>ajay2@ctopowered.com</t>
+  </si>
+  <si>
+    <t>ajay@arena.tec.br</t>
+  </si>
+  <si>
+    <t>ajay@daustin.co</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -407,11 +436,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBE00F2A-6AFA-4280-80FE-507041712647}">
-  <dimension ref="A1:A7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -455,16 +484,57 @@
         <v>6</v>
       </c>
     </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>16</v>
+      </c>
+    </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A1" r:id="rId1" xr:uid="{79872A69-DE12-4F94-9F53-D6EDBB3CE5BF}"/>
-    <hyperlink ref="A2" r:id="rId2" xr:uid="{0CF3EC1C-65AE-48BF-BBBB-E6049D6B865C}"/>
-    <hyperlink ref="A3" r:id="rId3" xr:uid="{195BD25E-F2E6-459C-BB04-DA5B89DAE536}"/>
-    <hyperlink ref="A4" r:id="rId4" xr:uid="{C1BF841C-B7D2-44E2-9B34-E6F753BA837F}"/>
-    <hyperlink ref="A5" r:id="rId5" xr:uid="{7CA69942-3CD9-49B5-ABA5-533C1BDA30AA}"/>
-    <hyperlink ref="A6" r:id="rId6" xr:uid="{23CF9CE9-E949-4DF4-A876-5E224414BE41}"/>
-    <hyperlink ref="A7" r:id="rId7" xr:uid="{100A532B-F0CE-466A-9310-31E6CE46901A}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>